<commit_message>
Actualizacion del cronograma y Hoja de desempeño
</commit_message>
<xml_diff>
--- a/P3GA1/DocumentosProyecto/Cronograma GA1.xlsx
+++ b/P3GA1/DocumentosProyecto/Cronograma GA1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\P\P3GA1\Prototipo_2P-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\P\P3GA1\DocumentosProyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D08EDF-5737-4A24-9754-F4FE3767182C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCD80EA-FC0E-4497-9A7E-32B90C7E0943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,7 +852,7 @@
         <v>43965</v>
       </c>
       <c r="H16" s="6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1044,13 +1044,13 @@
         <v>43965</v>
       </c>
       <c r="H24" s="6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H25" s="7">
         <f>AVERAGE(H3:H24)</f>
-        <v>0.99090909090909074</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reparando error encontrado por el ingeniero
</commit_message>
<xml_diff>
--- a/P3GA1/DocumentosProyecto/Cronograma GA1.xlsx
+++ b/P3GA1/DocumentosProyecto/Cronograma GA1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos_Git\SUI_AL2\P3GA1\DocumentosProyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBAS\Desktop\P\P3GA1\DocumentosProyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6EB4D0-F7FD-4038-82C8-DBA2DF63825F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -187,7 +188,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,14 +372,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,6 +412,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,974 +698,974 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.77734375" customWidth="1"/>
-    <col min="3" max="3" width="49.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="E4" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
         <f>+E4+F4</f>
         <v>43963</v>
       </c>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="8">
+      <c r="H4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="E5" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
         <f t="shared" ref="G5:G25" si="0">+E5+F5</f>
         <v>43963</v>
       </c>
-      <c r="H5" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="8">
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
+      <c r="E6" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H7" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="8">
+      <c r="E7" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
         <v>5</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H8" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="8">
+      <c r="E8" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
         <v>6</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="E9" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H9" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="8">
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="E10" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H10" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="8">
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="E11" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="8">
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="E12" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H12" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="8">
+      <c r="H12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
         <v>10</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>43964</v>
       </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H13" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="8">
+      <c r="H13" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <v>11</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H14" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="8">
+      <c r="E14" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
         <v>12</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="E15" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F15" s="6">
         <v>2</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="9">
         <f t="shared" si="0"/>
         <v>43965</v>
       </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="8">
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>43964</v>
       </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H16" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
+      <c r="H16" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <v>43965</v>
       </c>
-      <c r="F17" s="8">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
         <f t="shared" si="0"/>
         <v>43965</v>
       </c>
-      <c r="H17" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="8">
+      <c r="H17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
         <v>15</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H18" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="8">
+      <c r="E18" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
         <v>16</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H19" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="8">
+      <c r="E19" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="6">
         <v>17</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-      <c r="G20" s="11">
+      <c r="E20" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F20" s="6">
+        <v>1</v>
+      </c>
+      <c r="G20" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H20" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="8">
+      <c r="H20" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
         <v>18</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="8">
+      <c r="E21" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="6">
         <v>19</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H22" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="8">
+      <c r="E22" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="6">
         <v>20</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="11">
+      <c r="E23" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9">
         <f t="shared" si="0"/>
         <v>43964</v>
       </c>
-      <c r="H23" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="8">
+      <c r="H23" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
         <v>21</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0</v>
-      </c>
-      <c r="G24" s="11">
-        <f t="shared" si="0"/>
-        <v>43963</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="8">
+      <c r="E24" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="0"/>
+        <v>43963</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
         <v>22</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="10">
-        <v>43963</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="E25" s="8">
+        <v>43963</v>
+      </c>
+      <c r="F25" s="6">
         <v>2</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="9">
         <f t="shared" si="0"/>
         <v>43965</v>
       </c>
-      <c r="H25" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5" t="s">
+      <c r="H25" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="8">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
         <f>B25+1</f>
         <v>23</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="8">
         <v>43967</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="6">
         <f>G27-E27</f>
         <v>2</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="9">
         <v>43969</v>
       </c>
-      <c r="H27" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="8">
+      <c r="H27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="6">
         <f>B27+1</f>
         <v>24</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="8">
         <v>43968</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <f t="shared" ref="F28:F40" si="1">G28-E28</f>
         <v>0</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="9">
         <v>43968</v>
       </c>
-      <c r="H28" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="8">
+      <c r="H28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
         <f t="shared" ref="B29:B36" si="2">B28+1</f>
         <v>25</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="8">
         <v>43968</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="9">
         <v>43969</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="10">
         <v>1</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="8">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="6">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="8">
         <v>43968</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="6">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="9">
         <v>43969</v>
       </c>
-      <c r="H30" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="8">
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="8">
         <v>43969</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="9">
         <v>43969</v>
       </c>
-      <c r="H31" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="8">
+      <c r="H31" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="8">
         <v>43970</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="9">
         <v>43970</v>
       </c>
-      <c r="H32" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="8">
+      <c r="H32" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="8">
         <v>43971</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="9">
         <v>43971</v>
       </c>
-      <c r="H33" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="8">
+      <c r="H33" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="8">
         <v>43971</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="9">
         <v>43971</v>
       </c>
-      <c r="H34" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="8">
+      <c r="H34" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E35" s="8">
         <v>43971</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="9">
         <v>43971</v>
       </c>
-      <c r="H35" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="8">
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="8">
         <v>43972</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="9">
         <v>43972</v>
       </c>
-      <c r="H36" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="8">
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <f>B36+1</f>
         <v>33</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="8">
         <v>43972</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="9">
         <v>43972</v>
       </c>
-      <c r="H37" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="8">
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
         <f t="shared" ref="B38:B40" si="3">B37+1</f>
         <v>34</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="8">
         <v>43972</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="9">
         <v>43972</v>
       </c>
-      <c r="H38" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="8">
+      <c r="H38" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="8">
         <v>43972</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="9">
         <v>43972</v>
       </c>
-      <c r="H39" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="13">
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="11">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <v>43972</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G40" s="16">
+      <c r="G40" s="14">
         <v>43972</v>
       </c>
-      <c r="H40" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E42" s="2" t="s">
+      <c r="H40" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E42" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="3">
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="2">
         <f>AVERAGE(H4:H40)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D45" s="18" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D45" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E45" s="19">
+      <c r="E45" s="17">
         <f>+E4</f>
         <v>43963</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D46" s="18" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D46" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="19">
+      <c r="E46" s="17">
         <f>+G40</f>
         <v>43972</v>
       </c>

</xml_diff>